<commit_message>
updating for eventual use of fuzzy search
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Cristian Goodhart/Cristian Goodhart_2025-05-02_0.xlsx
+++ b/prep_and_checklists/Cristian Goodhart/Cristian Goodhart_2025-05-02_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Cristian Goodhart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B91290-749A-F740-BB78-6B50B5F80B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D937E1-3661-4749-94A3-3ECDE930C0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Cristian Goodhart 80 Guests 12:15 PM - 2:15 PM Saturday, May 10, 2025</t>
   </si>
@@ -120,6 +120,27 @@
   </si>
   <si>
     <t>3lbs</t>
+  </si>
+  <si>
+    <t>yogurt</t>
+  </si>
+  <si>
+    <t>red onion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> beefsteak tomato</t>
+  </si>
+  <si>
+    <t>1 case</t>
+  </si>
+  <si>
+    <t>5lbs</t>
+  </si>
+  <si>
+    <t>1 flat</t>
+  </si>
+  <si>
+    <t>2 x 3lbs</t>
   </si>
 </sst>
 </file>
@@ -196,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -205,6 +226,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +529,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -662,18 +687,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="93" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
@@ -685,7 +722,89 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>